<commit_message>
Creat liability_returns report, calculate aggregate liability return, and format asset liability returns table
</commit_message>
<xml_diff>
--- a/data/time_series/plan_mkt_value_data.xlsx
+++ b/data/time_series/plan_mkt_value_data.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maddi\Documents\UPS_MV\data\time_series\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E16FCF-086F-4DE3-A425-CEEF8E9AE040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB3E8A7-7240-4F2E-87A0-71D72628BABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IBT" sheetId="1" r:id="rId1"/>
     <sheet name="Pension" sheetId="2" r:id="rId2"/>
     <sheet name="Retirement" sheetId="3" r:id="rId3"/>
+    <sheet name="Total" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="2">
   <si>
     <t>Market Value</t>
   </si>
@@ -461,7 +462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C147"/>
   <sheetViews>
-    <sheetView topLeftCell="A123" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F144" sqref="F144"/>
     </sheetView>
   </sheetViews>
@@ -1658,7 +1659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABBA9FD4-CF43-40AB-9D8A-6D8C9591E0D3}">
   <dimension ref="A1:B146"/>
   <sheetViews>
-    <sheetView topLeftCell="A132" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D150" sqref="D150"/>
     </sheetView>
   </sheetViews>
@@ -2843,10 +2844,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34693692-6C77-4BB4-A99D-61623299D4F5}">
-  <dimension ref="A1:C147"/>
+  <dimension ref="A1:C150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4030,6 +4031,1351 @@
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C147" s="4"/>
     </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B150" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE1F9BAA-C331-4130-A1A0-9E94D0489A41}">
+  <dimension ref="A1:C150"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>40178</v>
+      </c>
+      <c r="B2" s="4">
+        <f>SUM(IBT!B2,Pension!B2,Retirement!B2)</f>
+        <v>15633809775.07</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>40209</v>
+      </c>
+      <c r="B3" s="4">
+        <f>SUM(IBT!B3,Pension!B3,Retirement!B3)</f>
+        <v>15489729218.43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>40237</v>
+      </c>
+      <c r="B4" s="4">
+        <f>SUM(IBT!B4,Pension!B4,Retirement!B4)</f>
+        <v>15775048697.139999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>40268</v>
+      </c>
+      <c r="B5" s="4">
+        <f>SUM(IBT!B5,Pension!B5,Retirement!B5)</f>
+        <v>16704873758.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>40298</v>
+      </c>
+      <c r="B6" s="4">
+        <f>SUM(IBT!B6,Pension!B6,Retirement!B6)</f>
+        <v>17132130003.51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>40329</v>
+      </c>
+      <c r="B7" s="4">
+        <f>SUM(IBT!B7,Pension!B7,Retirement!B7)</f>
+        <v>16351241876.799999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>40359</v>
+      </c>
+      <c r="B8" s="4">
+        <f>SUM(IBT!B8,Pension!B8,Retirement!B8)</f>
+        <v>16127227316.289999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>40390</v>
+      </c>
+      <c r="B9" s="4">
+        <f>SUM(IBT!B9,Pension!B9,Retirement!B9)</f>
+        <v>16894210925.619999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>40421</v>
+      </c>
+      <c r="B10" s="4">
+        <f>SUM(IBT!B10,Pension!B10,Retirement!B10)</f>
+        <v>16864762411.98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>40451</v>
+      </c>
+      <c r="B11" s="4">
+        <f>SUM(IBT!B11,Pension!B11,Retirement!B11)</f>
+        <v>17683853962.580002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>40482</v>
+      </c>
+      <c r="B12" s="4">
+        <f>SUM(IBT!B12,Pension!B12,Retirement!B12)</f>
+        <v>17795005221.620003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <v>40512</v>
+      </c>
+      <c r="B13" s="4">
+        <f>SUM(IBT!B13,Pension!B13,Retirement!B13)</f>
+        <v>19628314376.709999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="2">
+        <v>40543</v>
+      </c>
+      <c r="B14" s="4">
+        <f>SUM(IBT!B14,Pension!B14,Retirement!B14)</f>
+        <v>20035126948.73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
+        <v>40574</v>
+      </c>
+      <c r="B15" s="4">
+        <f>SUM(IBT!B15,Pension!B15,Retirement!B15)</f>
+        <v>21163701726.799999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>40602</v>
+      </c>
+      <c r="B16" s="4">
+        <f>SUM(IBT!B16,Pension!B16,Retirement!B16)</f>
+        <v>21592868236.349998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
+        <v>40633</v>
+      </c>
+      <c r="B17" s="4">
+        <f>SUM(IBT!B17,Pension!B17,Retirement!B17)</f>
+        <v>21597393553.599998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
+        <v>40663</v>
+      </c>
+      <c r="B18" s="4">
+        <f>SUM(IBT!B18,Pension!B18,Retirement!B18)</f>
+        <v>22196442158.830002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="2">
+        <v>40694</v>
+      </c>
+      <c r="B19" s="4">
+        <f>SUM(IBT!B19,Pension!B19,Retirement!B19)</f>
+        <v>22284623894.07</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="2">
+        <v>40724</v>
+      </c>
+      <c r="B20" s="4">
+        <f>SUM(IBT!B20,Pension!B20,Retirement!B20)</f>
+        <v>21869129586.239998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="2">
+        <v>40755</v>
+      </c>
+      <c r="B21" s="4">
+        <f>SUM(IBT!B21,Pension!B21,Retirement!B21)</f>
+        <v>22052015022.439999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="2">
+        <v>40786</v>
+      </c>
+      <c r="B22" s="4">
+        <f>SUM(IBT!B22,Pension!B22,Retirement!B22)</f>
+        <v>21857152498.610001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="2">
+        <v>40816</v>
+      </c>
+      <c r="B23" s="4">
+        <f>SUM(IBT!B23,Pension!B23,Retirement!B23)</f>
+        <v>21890587182.540001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="2">
+        <v>40847</v>
+      </c>
+      <c r="B24" s="4">
+        <f>SUM(IBT!B24,Pension!B24,Retirement!B24)</f>
+        <v>22617832290.32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="2">
+        <v>40877</v>
+      </c>
+      <c r="B25" s="4">
+        <f>SUM(IBT!B25,Pension!B25,Retirement!B25)</f>
+        <v>22404660643.810001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="2">
+        <v>40908</v>
+      </c>
+      <c r="B26" s="4">
+        <f>SUM(IBT!B26,Pension!B26,Retirement!B26)</f>
+        <v>22610566714.970001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="2">
+        <v>40939</v>
+      </c>
+      <c r="B27" s="4">
+        <f>SUM(IBT!B27,Pension!B27,Retirement!B27)</f>
+        <v>23182541487.510002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="2">
+        <v>40968</v>
+      </c>
+      <c r="B28" s="4">
+        <f>SUM(IBT!B28,Pension!B28,Retirement!B28)</f>
+        <v>23538890877.400002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="2">
+        <v>40999</v>
+      </c>
+      <c r="B29" s="4">
+        <f>SUM(IBT!B29,Pension!B29,Retirement!B29)</f>
+        <v>23568457835.099998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="2">
+        <v>41029</v>
+      </c>
+      <c r="B30" s="4">
+        <f>SUM(IBT!B30,Pension!B30,Retirement!B30)</f>
+        <v>23750894239.669998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="2">
+        <v>41060</v>
+      </c>
+      <c r="B31" s="4">
+        <f>SUM(IBT!B31,Pension!B31,Retirement!B31)</f>
+        <v>23525188092.25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="2">
+        <v>41090</v>
+      </c>
+      <c r="B32" s="4">
+        <f>SUM(IBT!B32,Pension!B32,Retirement!B32)</f>
+        <v>23966952669.709999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="2">
+        <v>41121</v>
+      </c>
+      <c r="B33" s="4">
+        <f>SUM(IBT!B33,Pension!B33,Retirement!B33)</f>
+        <v>24445028323.779999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="2">
+        <v>41152</v>
+      </c>
+      <c r="B34" s="4">
+        <f>SUM(IBT!B34,Pension!B34,Retirement!B34)</f>
+        <v>24546173849.48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="2">
+        <v>41182</v>
+      </c>
+      <c r="B35" s="4">
+        <f>SUM(IBT!B35,Pension!B35,Retirement!B35)</f>
+        <v>24697695785.049999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="2">
+        <v>41213</v>
+      </c>
+      <c r="B36" s="4">
+        <f>SUM(IBT!B36,Pension!B36,Retirement!B36)</f>
+        <v>24675625120.169998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" s="2">
+        <v>41243</v>
+      </c>
+      <c r="B37" s="4">
+        <f>SUM(IBT!B37,Pension!B37,Retirement!B37)</f>
+        <v>24802249901.279999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" s="2">
+        <v>41274</v>
+      </c>
+      <c r="B38" s="4">
+        <f>SUM(IBT!B38,Pension!B38,Retirement!B38)</f>
+        <v>24895725823.459999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" s="2">
+        <v>41305</v>
+      </c>
+      <c r="B39" s="4">
+        <f>SUM(IBT!B39,Pension!B39,Retirement!B39)</f>
+        <v>25170361391.66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" s="2">
+        <v>41333</v>
+      </c>
+      <c r="B40" s="4">
+        <f>SUM(IBT!B40,Pension!B40,Retirement!B40)</f>
+        <v>25279056931.75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" s="2">
+        <v>41364</v>
+      </c>
+      <c r="B41" s="4">
+        <f>SUM(IBT!B41,Pension!B41,Retirement!B41)</f>
+        <v>25595461395.489998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" s="2">
+        <v>41394</v>
+      </c>
+      <c r="B42" s="4">
+        <f>SUM(IBT!B42,Pension!B42,Retirement!B42)</f>
+        <v>26172807411.43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" s="2">
+        <v>41425</v>
+      </c>
+      <c r="B43" s="4">
+        <f>SUM(IBT!B43,Pension!B43,Retirement!B43)</f>
+        <v>25673836920.309998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" s="2">
+        <v>41455</v>
+      </c>
+      <c r="B44" s="4">
+        <f>SUM(IBT!B44,Pension!B44,Retirement!B44)</f>
+        <v>25144097226.379997</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" s="2">
+        <v>41486</v>
+      </c>
+      <c r="B45" s="4">
+        <f>SUM(IBT!B45,Pension!B45,Retirement!B45)</f>
+        <v>25436535483.029999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" s="2">
+        <v>41517</v>
+      </c>
+      <c r="B46" s="4">
+        <f>SUM(IBT!B46,Pension!B46,Retirement!B46)</f>
+        <v>25090551978.139999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" s="2">
+        <v>41547</v>
+      </c>
+      <c r="B47" s="4">
+        <f>SUM(IBT!B47,Pension!B47,Retirement!B47)</f>
+        <v>25528342822.260002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" s="2">
+        <v>41578</v>
+      </c>
+      <c r="B48" s="4">
+        <f>SUM(IBT!B48,Pension!B48,Retirement!B48)</f>
+        <v>26027210514.610001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" s="2">
+        <v>41608</v>
+      </c>
+      <c r="B49" s="4">
+        <f>SUM(IBT!B49,Pension!B49,Retirement!B49)</f>
+        <v>26003668184.25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" s="2">
+        <v>41639</v>
+      </c>
+      <c r="B50" s="4">
+        <f>SUM(IBT!B50,Pension!B50,Retirement!B50)</f>
+        <v>26126136558.370003</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" s="2">
+        <v>41670</v>
+      </c>
+      <c r="B51" s="4">
+        <f>SUM(IBT!B51,Pension!B51,Retirement!B51)</f>
+        <v>26107545286.209999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" s="2">
+        <v>41698</v>
+      </c>
+      <c r="B52" s="4">
+        <f>SUM(IBT!B52,Pension!B52,Retirement!B52)</f>
+        <v>26638014657</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" s="2">
+        <v>41729</v>
+      </c>
+      <c r="B53" s="4">
+        <f>SUM(IBT!B53,Pension!B53,Retirement!B53)</f>
+        <v>26769907188.32</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" s="2">
+        <v>41759</v>
+      </c>
+      <c r="B54" s="4">
+        <f>SUM(IBT!B54,Pension!B54,Retirement!B54)</f>
+        <v>26765961123.209999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" s="2">
+        <v>41790</v>
+      </c>
+      <c r="B55" s="4">
+        <f>SUM(IBT!B55,Pension!B55,Retirement!B55)</f>
+        <v>27191839755.379997</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" s="2">
+        <v>41820</v>
+      </c>
+      <c r="B56" s="4">
+        <f>SUM(IBT!B56,Pension!B56,Retirement!B56)</f>
+        <v>27325539811.990002</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" s="2">
+        <v>41851</v>
+      </c>
+      <c r="B57" s="4">
+        <f>SUM(IBT!B57,Pension!B57,Retirement!B57)</f>
+        <v>27156693166.089996</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" s="2">
+        <v>41882</v>
+      </c>
+      <c r="B58" s="4">
+        <f>SUM(IBT!B58,Pension!B58,Retirement!B58)</f>
+        <v>27744061638.859997</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" s="2">
+        <v>41912</v>
+      </c>
+      <c r="B59" s="4">
+        <f>SUM(IBT!B59,Pension!B59,Retirement!B59)</f>
+        <v>27150516717.209999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" s="2">
+        <v>41943</v>
+      </c>
+      <c r="B60" s="4">
+        <f>SUM(IBT!B60,Pension!B60,Retirement!B60)</f>
+        <v>27371582530.760002</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" s="2">
+        <v>41973</v>
+      </c>
+      <c r="B61" s="4">
+        <f>SUM(IBT!B61,Pension!B61,Retirement!B61)</f>
+        <v>27755791534.099998</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" s="2">
+        <v>42004</v>
+      </c>
+      <c r="B62" s="4">
+        <f>SUM(IBT!B62,Pension!B62,Retirement!B62)</f>
+        <v>28782286672.540001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" s="2">
+        <v>42035</v>
+      </c>
+      <c r="B63" s="4">
+        <f>SUM(IBT!B63,Pension!B63,Retirement!B63)</f>
+        <v>29377893373.27</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" s="2">
+        <v>42063</v>
+      </c>
+      <c r="B64" s="4">
+        <f>SUM(IBT!B64,Pension!B64,Retirement!B64)</f>
+        <v>29527582270.599998</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" s="2">
+        <v>42094</v>
+      </c>
+      <c r="B65" s="4">
+        <f>SUM(IBT!B65,Pension!B65,Retirement!B65)</f>
+        <v>29472066114.919998</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" s="2">
+        <v>42124</v>
+      </c>
+      <c r="B66" s="4">
+        <f>SUM(IBT!B66,Pension!B66,Retirement!B66)</f>
+        <v>29408499309.230003</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" s="2">
+        <v>42155</v>
+      </c>
+      <c r="B67" s="4">
+        <f>SUM(IBT!B67,Pension!B67,Retirement!B67)</f>
+        <v>29287873259.310001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68" s="2">
+        <v>42185</v>
+      </c>
+      <c r="B68" s="4">
+        <f>SUM(IBT!B68,Pension!B68,Retirement!B68)</f>
+        <v>28649880311.460003</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" s="2">
+        <v>42216</v>
+      </c>
+      <c r="B69" s="4">
+        <f>SUM(IBT!B69,Pension!B69,Retirement!B69)</f>
+        <v>28876049490.889999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" s="2">
+        <v>42247</v>
+      </c>
+      <c r="B70" s="4">
+        <f>SUM(IBT!B70,Pension!B70,Retirement!B70)</f>
+        <v>28013794466.529999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" s="2">
+        <v>42277</v>
+      </c>
+      <c r="B71" s="4">
+        <f>SUM(IBT!B71,Pension!B71,Retirement!B71)</f>
+        <v>27687481033.779999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72" s="2">
+        <v>42308</v>
+      </c>
+      <c r="B72" s="4">
+        <f>SUM(IBT!B72,Pension!B72,Retirement!B72)</f>
+        <v>28326214032.700001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73" s="2">
+        <v>42338</v>
+      </c>
+      <c r="B73" s="4">
+        <f>SUM(IBT!B73,Pension!B73,Retirement!B73)</f>
+        <v>28136428854.080002</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74" s="2">
+        <v>42369</v>
+      </c>
+      <c r="B74" s="4">
+        <f>SUM(IBT!B74,Pension!B74,Retirement!B74)</f>
+        <v>28846123319.360001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A75" s="2">
+        <v>42400</v>
+      </c>
+      <c r="B75" s="4">
+        <f>SUM(IBT!B75,Pension!B75,Retirement!B75)</f>
+        <v>28336242435.290001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A76" s="2">
+        <v>42429</v>
+      </c>
+      <c r="B76" s="4">
+        <f>SUM(IBT!B76,Pension!B76,Retirement!B76)</f>
+        <v>28455548735.700001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77" s="2">
+        <v>42460</v>
+      </c>
+      <c r="B77" s="4">
+        <f>SUM(IBT!B77,Pension!B77,Retirement!B77)</f>
+        <v>29356543183.02</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A78" s="2">
+        <v>42490</v>
+      </c>
+      <c r="B78" s="4">
+        <f>SUM(IBT!B78,Pension!B78,Retirement!B78)</f>
+        <v>29541899253.779999</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A79" s="2">
+        <v>42521</v>
+      </c>
+      <c r="B79" s="4">
+        <f>SUM(IBT!B79,Pension!B79,Retirement!B79)</f>
+        <v>29511294102.970001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A80" s="2">
+        <v>42551</v>
+      </c>
+      <c r="B80" s="4">
+        <f>SUM(IBT!B80,Pension!B80,Retirement!B80)</f>
+        <v>29721707293.18</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A81" s="2">
+        <v>42582</v>
+      </c>
+      <c r="B81" s="4">
+        <f>SUM(IBT!B81,Pension!B81,Retirement!B81)</f>
+        <v>30265017930.439999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A82" s="2">
+        <v>42613</v>
+      </c>
+      <c r="B82" s="4">
+        <f>SUM(IBT!B82,Pension!B82,Retirement!B82)</f>
+        <v>30212130836.659996</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83" s="2">
+        <v>42643</v>
+      </c>
+      <c r="B83" s="4">
+        <f>SUM(IBT!B83,Pension!B83,Retirement!B83)</f>
+        <v>31311065698.300003</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A84" s="2">
+        <v>42674</v>
+      </c>
+      <c r="B84" s="4">
+        <f>SUM(IBT!B84,Pension!B84,Retirement!B84)</f>
+        <v>30735579110.59</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85" s="2">
+        <v>42704</v>
+      </c>
+      <c r="B85" s="4">
+        <f>SUM(IBT!B85,Pension!B85,Retirement!B85)</f>
+        <v>30294027553</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A86" s="2">
+        <v>42735</v>
+      </c>
+      <c r="B86" s="4">
+        <f>SUM(IBT!B86,Pension!B86,Retirement!B86)</f>
+        <v>31134438714.84</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A87" s="2">
+        <v>42766</v>
+      </c>
+      <c r="B87" s="4">
+        <f>SUM(IBT!B87,Pension!B87,Retirement!B87)</f>
+        <v>31406508587.93</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88" s="2">
+        <v>42794</v>
+      </c>
+      <c r="B88" s="4">
+        <f>SUM(IBT!B88,Pension!B88,Retirement!B88)</f>
+        <v>31862808989.720001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A89" s="2">
+        <v>42825</v>
+      </c>
+      <c r="B89" s="4">
+        <f>SUM(IBT!B89,Pension!B89,Retirement!B89)</f>
+        <v>34237099341.939999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A90" s="2">
+        <v>42855</v>
+      </c>
+      <c r="B90" s="4">
+        <f>SUM(IBT!B90,Pension!B90,Retirement!B90)</f>
+        <v>34601102374.349998</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A91" s="2">
+        <v>42886</v>
+      </c>
+      <c r="B91" s="4">
+        <f>SUM(IBT!B91,Pension!B91,Retirement!B91)</f>
+        <v>35025362965.57</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A92" s="2">
+        <v>42916</v>
+      </c>
+      <c r="B92" s="4">
+        <f>SUM(IBT!B92,Pension!B92,Retirement!B92)</f>
+        <v>35106467417.43</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A93" s="2">
+        <v>42947</v>
+      </c>
+      <c r="B93" s="4">
+        <f>SUM(IBT!B93,Pension!B93,Retirement!B93)</f>
+        <v>35405676882.5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A94" s="2">
+        <v>42978</v>
+      </c>
+      <c r="B94" s="4">
+        <f>SUM(IBT!B94,Pension!B94,Retirement!B94)</f>
+        <v>35685401140.059998</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A95" s="2">
+        <v>43008</v>
+      </c>
+      <c r="B95" s="4">
+        <f>SUM(IBT!B95,Pension!B95,Retirement!B95)</f>
+        <v>35874830645.559998</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96" s="2">
+        <v>43039</v>
+      </c>
+      <c r="B96" s="4">
+        <f>SUM(IBT!B96,Pension!B96,Retirement!B96)</f>
+        <v>36114807334.970001</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A97" s="2">
+        <v>43069</v>
+      </c>
+      <c r="B97" s="4">
+        <f>SUM(IBT!B97,Pension!B97,Retirement!B97)</f>
+        <v>36495501947.440002</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A98" s="2">
+        <v>43100</v>
+      </c>
+      <c r="B98" s="4">
+        <f>SUM(IBT!B98,Pension!B98,Retirement!B98)</f>
+        <v>41855947325.630005</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A99" s="2">
+        <v>43131</v>
+      </c>
+      <c r="B99" s="4">
+        <f>SUM(IBT!B99,Pension!B99,Retirement!B99)</f>
+        <v>42583608483.910004</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A100" s="2">
+        <v>43159</v>
+      </c>
+      <c r="B100" s="4">
+        <f>SUM(IBT!B100,Pension!B100,Retirement!B100)</f>
+        <v>41211539283.339996</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A101" s="2">
+        <v>43190</v>
+      </c>
+      <c r="B101" s="4">
+        <f>SUM(IBT!B101,Pension!B101,Retirement!B101)</f>
+        <v>41345361923.699997</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A102" s="2">
+        <v>43220</v>
+      </c>
+      <c r="B102" s="4">
+        <f>SUM(IBT!B102,Pension!B102,Retirement!B102)</f>
+        <v>41046653376.559998</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A103" s="2">
+        <v>43251</v>
+      </c>
+      <c r="B103" s="4">
+        <f>SUM(IBT!B103,Pension!B103,Retirement!B103)</f>
+        <v>41313125652.080002</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A104" s="2">
+        <v>43281</v>
+      </c>
+      <c r="B104" s="4">
+        <f>SUM(IBT!B104,Pension!B104,Retirement!B104)</f>
+        <v>41120926179.029999</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A105" s="2">
+        <v>43312</v>
+      </c>
+      <c r="B105" s="4">
+        <f>SUM(IBT!B105,Pension!B105,Retirement!B105)</f>
+        <v>41384483579.770004</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A106" s="2">
+        <v>43343</v>
+      </c>
+      <c r="B106" s="4">
+        <f>SUM(IBT!B106,Pension!B106,Retirement!B106)</f>
+        <v>41662699191.550003</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A107" s="2">
+        <v>43373</v>
+      </c>
+      <c r="B107" s="4">
+        <f>SUM(IBT!B107,Pension!B107,Retirement!B107)</f>
+        <v>41186844593.330002</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A108" s="2">
+        <v>43404</v>
+      </c>
+      <c r="B108" s="4">
+        <f>SUM(IBT!B108,Pension!B108,Retirement!B108)</f>
+        <v>39382932997.410004</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A109" s="2">
+        <v>43434</v>
+      </c>
+      <c r="B109" s="4">
+        <f>SUM(IBT!B109,Pension!B109,Retirement!B109)</f>
+        <v>39775062674.709999</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A110" s="2">
+        <v>43465</v>
+      </c>
+      <c r="B110" s="4">
+        <f>SUM(IBT!B110,Pension!B110,Retirement!B110)</f>
+        <v>39522884974.100006</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A111" s="2">
+        <v>43496</v>
+      </c>
+      <c r="B111" s="4">
+        <f>SUM(IBT!B111,Pension!B111,Retirement!B111)</f>
+        <v>40669954095.649994</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A112" s="2">
+        <v>43524</v>
+      </c>
+      <c r="B112" s="4">
+        <f>SUM(IBT!B112,Pension!B112,Retirement!B112)</f>
+        <v>40797714345.529999</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A113" s="2">
+        <v>43555</v>
+      </c>
+      <c r="B113" s="4">
+        <f>SUM(IBT!B113,Pension!B113,Retirement!B113)</f>
+        <v>41816004324.669998</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A114" s="2">
+        <v>43585</v>
+      </c>
+      <c r="B114" s="4">
+        <f>SUM(IBT!B114,Pension!B114,Retirement!B114)</f>
+        <v>42743010048.029999</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A115" s="2">
+        <v>43616</v>
+      </c>
+      <c r="B115" s="4">
+        <f>SUM(IBT!B115,Pension!B115,Retirement!B115)</f>
+        <v>43049509347.520004</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A116" s="2">
+        <v>43646</v>
+      </c>
+      <c r="B116" s="4">
+        <f>SUM(IBT!B116,Pension!B116,Retirement!B116)</f>
+        <v>44201801916.779999</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A117" s="2">
+        <v>43677</v>
+      </c>
+      <c r="B117" s="4">
+        <f>SUM(IBT!B117,Pension!B117,Retirement!B117)</f>
+        <v>44289184114.949997</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A118" s="2">
+        <v>43708</v>
+      </c>
+      <c r="B118" s="4">
+        <f>SUM(IBT!B118,Pension!B118,Retirement!B118)</f>
+        <v>46120218348.729996</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A119" s="2">
+        <v>43738</v>
+      </c>
+      <c r="B119" s="4">
+        <f>SUM(IBT!B119,Pension!B119,Retirement!B119)</f>
+        <v>46949500920.5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A120" s="2">
+        <v>43769</v>
+      </c>
+      <c r="B120" s="4">
+        <f>SUM(IBT!B120,Pension!B120,Retirement!B120)</f>
+        <v>46865616845.860001</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A121" s="2">
+        <v>43799</v>
+      </c>
+      <c r="B121" s="4">
+        <f>SUM(IBT!B121,Pension!B121,Retirement!B121)</f>
+        <v>47123526214.259995</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A122" s="2">
+        <v>43830</v>
+      </c>
+      <c r="B122" s="4">
+        <f>SUM(IBT!B122,Pension!B122,Retirement!B122)</f>
+        <v>46141543427.790001</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A123" s="2">
+        <v>43861</v>
+      </c>
+      <c r="B123" s="4">
+        <f>SUM(IBT!B123,Pension!B123,Retirement!B123)</f>
+        <v>47197571777.949997</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A124" s="2">
+        <v>43890</v>
+      </c>
+      <c r="B124" s="4">
+        <f>SUM(IBT!B124,Pension!B124,Retirement!B124)</f>
+        <v>47123736418.860001</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A125" s="2">
+        <v>43921</v>
+      </c>
+      <c r="B125" s="4">
+        <f>SUM(IBT!B125,Pension!B125,Retirement!B125)</f>
+        <v>45203938859.300003</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A126" s="2">
+        <v>43951</v>
+      </c>
+      <c r="B126" s="4">
+        <f>SUM(IBT!B126,Pension!B126,Retirement!B126)</f>
+        <v>47063924664.940002</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A127" s="2">
+        <v>43982</v>
+      </c>
+      <c r="B127" s="4">
+        <f>SUM(IBT!B127,Pension!B127,Retirement!B127)</f>
+        <v>47081053140.339996</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A128" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B128" s="4">
+        <f>SUM(IBT!B128,Pension!B128,Retirement!B128)</f>
+        <v>47426479912.610001</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A129" s="2">
+        <v>44043</v>
+      </c>
+      <c r="B129" s="4">
+        <f>SUM(IBT!B129,Pension!B129,Retirement!B129)</f>
+        <v>49195581002.360001</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A130" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B130" s="4">
+        <f>SUM(IBT!B130,Pension!B130,Retirement!B130)</f>
+        <v>48906000373.669998</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A131" s="2">
+        <v>44104</v>
+      </c>
+      <c r="B131" s="4">
+        <f>SUM(IBT!B131,Pension!B131,Retirement!B131)</f>
+        <v>49328610123.339996</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A132" s="2">
+        <v>44135</v>
+      </c>
+      <c r="B132" s="4">
+        <f>SUM(IBT!B132,Pension!B132,Retirement!B132)</f>
+        <v>48025973012.379997</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A133" s="2">
+        <v>44165</v>
+      </c>
+      <c r="B133" s="4">
+        <f>SUM(IBT!B133,Pension!B133,Retirement!B133)</f>
+        <v>50439922757.960007</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A134" s="2">
+        <v>44196</v>
+      </c>
+      <c r="B134" s="4">
+        <f>SUM(IBT!B134,Pension!B134,Retirement!B134)</f>
+        <v>52788406154.489998</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A135" s="2">
+        <v>44227</v>
+      </c>
+      <c r="B135" s="4">
+        <f>SUM(IBT!B135,Pension!B135,Retirement!B135)</f>
+        <v>51587924289.860001</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A136" s="2">
+        <v>44255</v>
+      </c>
+      <c r="B136" s="4">
+        <f>SUM(IBT!B136,Pension!B136,Retirement!B136)</f>
+        <v>50499267741.220001</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A137" s="2">
+        <v>44286</v>
+      </c>
+      <c r="B137" s="4">
+        <f>SUM(IBT!B137,Pension!B137,Retirement!B137)</f>
+        <v>50392639291.639999</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A138" s="2">
+        <v>44316</v>
+      </c>
+      <c r="B138" s="4">
+        <f>SUM(IBT!B138,Pension!B138,Retirement!B138)</f>
+        <v>51700906918.139999</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A139" s="2">
+        <v>44347</v>
+      </c>
+      <c r="B139" s="4">
+        <f>SUM(IBT!B139,Pension!B139,Retirement!B139)</f>
+        <v>52378479915.339996</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A140" s="2">
+        <v>44377</v>
+      </c>
+      <c r="B140" s="4">
+        <f>SUM(IBT!B140,Pension!B140,Retirement!B140)</f>
+        <v>53479086658.270004</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A141" s="2">
+        <v>44408</v>
+      </c>
+      <c r="B141" s="4">
+        <f>SUM(IBT!B141,Pension!B141,Retirement!B141)</f>
+        <v>54428674790.350006</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A142" s="2">
+        <v>44439</v>
+      </c>
+      <c r="B142" s="4">
+        <f>SUM(IBT!B142,Pension!B142,Retirement!B142)</f>
+        <v>54870263825.589996</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A143" s="2">
+        <v>44469</v>
+      </c>
+      <c r="B143" s="4">
+        <f>SUM(IBT!B143,Pension!B143,Retirement!B143)</f>
+        <v>52900976752.919998</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A144" s="2">
+        <v>44500</v>
+      </c>
+      <c r="B144" s="4">
+        <f>SUM(IBT!B144,Pension!B144,Retirement!B144)</f>
+        <v>54300695591.470001</v>
+      </c>
+      <c r="C144" s="4"/>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A145" s="2">
+        <v>44530</v>
+      </c>
+      <c r="B145" s="4">
+        <f>SUM(IBT!B145,Pension!B145,Retirement!B145)</f>
+        <v>55089285603.900002</v>
+      </c>
+      <c r="C145" s="4"/>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A146" s="2">
+        <v>44561</v>
+      </c>
+      <c r="B146" s="4">
+        <f>SUM(IBT!B146,Pension!B146,Retirement!B146)</f>
+        <v>55524799409.729996</v>
+      </c>
+      <c r="C146" s="4"/>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C147" s="4"/>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B150" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>